<commit_message>
Add info to graphs so people other than me might understand it
</commit_message>
<xml_diff>
--- a/PerformanceGraphs.xlsx
+++ b/PerformanceGraphs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="0" windowWidth="20505" windowHeight="9120"/>
+    <workbookView xWindow="2070" yWindow="0" windowWidth="20505" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Count</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>Log(Bulk)</t>
+  </si>
+  <si>
+    <t>* Parallel is the Simple case spanned to 32 parallel requests</t>
+  </si>
+  <si>
+    <t>* Bulk is a single thread, reading 32 keys in one SELECT query</t>
+  </si>
+  <si>
+    <t>* Time is in milliseconds</t>
   </si>
 </sst>
 </file>
@@ -437,11 +446,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="378784048"/>
-        <c:axId val="378784440"/>
+        <c:axId val="316406288"/>
+        <c:axId val="316405896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="378784048"/>
+        <c:axId val="316406288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,7 +493,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="378784440"/>
+        <c:crossAx val="316405896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -492,7 +501,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="378784440"/>
+        <c:axId val="316405896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -543,7 +552,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="378784048"/>
+        <c:crossAx val="316406288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1478,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="I23:Q29"/>
+  <dimension ref="I20:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1495,6 +1504,19 @@
     <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="20" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="23" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Get (f'ing crazy) perf results for writes
</commit_message>
<xml_diff>
--- a/PerformanceGraphs.xlsx
+++ b/PerformanceGraphs.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="0" windowWidth="20505" windowHeight="9120"/>
+    <workbookView xWindow="3105" yWindow="0" windowWidth="20505" windowHeight="9120" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ReadTests" sheetId="1" r:id="rId1"/>
+    <sheet name="WriteTests" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>Count</t>
   </si>
@@ -195,7 +196,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$23</c:f>
+              <c:f>ReadTests!$N$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -218,7 +219,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$I$24:$I$29</c:f>
+              <c:f>ReadTests!$I$24:$I$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -245,7 +246,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$24:$N$29</c:f>
+              <c:f>ReadTests!$N$24:$N$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -277,7 +278,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$23</c:f>
+              <c:f>ReadTests!$O$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -300,7 +301,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$24:$O$29</c:f>
+              <c:f>ReadTests!$O$24:$O$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -332,7 +333,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$23</c:f>
+              <c:f>ReadTests!$P$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -355,7 +356,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$24:$P$29</c:f>
+              <c:f>ReadTests!$P$24:$P$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -387,7 +388,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$23</c:f>
+              <c:f>ReadTests!$Q$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -410,7 +411,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$24:$Q$29</c:f>
+              <c:f>ReadTests!$Q$24:$Q$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -446,11 +447,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="316406288"/>
-        <c:axId val="316405896"/>
+        <c:axId val="241015312"/>
+        <c:axId val="241012960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="316406288"/>
+        <c:axId val="241015312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -493,7 +494,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316405896"/>
+        <c:crossAx val="241012960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -501,7 +502,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="316405896"/>
+        <c:axId val="241012960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -552,7 +553,526 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316406288"/>
+        <c:crossAx val="241015312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Write Performance (Log Scale)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>WriteTests!$N$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Log(Simple Time)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>WriteTests!$I$24:$I$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>WriteTests!$N$24:$N$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.6138418218760693</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3710678622717363</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1989318699322089</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.295083059251656</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.237531171569807</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3205031336851318</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>WriteTests!$O$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Log(Expected)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>WriteTests!$O$24:$O$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.3222192947339193</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3222192947339193</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3710678622717363</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3710678622717358</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3710678622717358</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3710678622717358</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>WriteTests!$P$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Log(Parallel)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>WriteTests!$P$24:$P$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.0969100130080562</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.271841606536499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1983821300082944</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.224895470849483</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2331383122024064</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.2153411481740353</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>WriteTests!$Q$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Log(Bulk)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>WriteTests!$Q$24:$Q$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.4297522800024081</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4313637641589874</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2304489213782739</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7853298350107671</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0496056125949731</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.2605722081234925</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="286410128"/>
+        <c:axId val="240764272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="286410128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="240764272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="240764272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="286410128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -673,7 +1193,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1208,6 +2284,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="8" name="Chart 7"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>233362</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1489,7 +2602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="I20:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+    <sheetView topLeftCell="K3" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -1752,4 +2865,273 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="I20:Q29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="L4" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="15.85546875" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="20" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23" t="s">
+        <v>2</v>
+      </c>
+      <c r="L23" t="s">
+        <v>6</v>
+      </c>
+      <c r="M23" t="s">
+        <v>7</v>
+      </c>
+      <c r="N23" t="s">
+        <v>4</v>
+      </c>
+      <c r="O23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P23" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>411</v>
+      </c>
+      <c r="K24">
+        <v>2.1</v>
+      </c>
+      <c r="L24">
+        <v>125</v>
+      </c>
+      <c r="M24">
+        <v>269</v>
+      </c>
+      <c r="N24">
+        <f>LOG(J24)</f>
+        <v>2.6138418218760693</v>
+      </c>
+      <c r="O24">
+        <f>LOG(K24)</f>
+        <v>0.3222192947339193</v>
+      </c>
+      <c r="P24">
+        <f>LOG(L24)</f>
+        <v>2.0969100130080562</v>
+      </c>
+      <c r="Q24">
+        <f>LOG(M24)</f>
+        <v>2.4297522800024081</v>
+      </c>
+    </row>
+    <row r="25" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>10</v>
+      </c>
+      <c r="J25">
+        <v>235</v>
+      </c>
+      <c r="K25">
+        <v>21</v>
+      </c>
+      <c r="L25">
+        <v>187</v>
+      </c>
+      <c r="M25">
+        <v>27</v>
+      </c>
+      <c r="N25">
+        <f>LOG(J25)</f>
+        <v>2.3710678622717363</v>
+      </c>
+      <c r="O25">
+        <f t="shared" ref="O25:Q29" si="0">LOG(K25)</f>
+        <v>1.3222192947339193</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="0"/>
+        <v>2.271841606536499</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="0"/>
+        <v>1.4313637641589874</v>
+      </c>
+    </row>
+    <row r="26" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>100</v>
+      </c>
+      <c r="J26">
+        <v>1581</v>
+      </c>
+      <c r="K26">
+        <f>J25*10</f>
+        <v>2350</v>
+      </c>
+      <c r="L26">
+        <v>1579</v>
+      </c>
+      <c r="M26">
+        <v>17</v>
+      </c>
+      <c r="N26">
+        <f>LOG(J26)</f>
+        <v>3.1989318699322089</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="0"/>
+        <v>3.3710678622717363</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="0"/>
+        <v>3.1983821300082944</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="0"/>
+        <v>1.2304489213782739</v>
+      </c>
+    </row>
+    <row r="27" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>1000</v>
+      </c>
+      <c r="J27">
+        <v>19728</v>
+      </c>
+      <c r="K27">
+        <f>K26*10</f>
+        <v>23500</v>
+      </c>
+      <c r="L27">
+        <v>16784</v>
+      </c>
+      <c r="M27">
+        <v>61</v>
+      </c>
+      <c r="N27">
+        <f>LOG(J27)</f>
+        <v>4.295083059251656</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="0"/>
+        <v>4.3710678622717358</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="0"/>
+        <v>4.224895470849483</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="0"/>
+        <v>1.7853298350107671</v>
+      </c>
+    </row>
+    <row r="28" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>10000</v>
+      </c>
+      <c r="J28">
+        <v>172795</v>
+      </c>
+      <c r="K28">
+        <f t="shared" ref="K28:K29" si="1">K27*10</f>
+        <v>235000</v>
+      </c>
+      <c r="L28">
+        <v>171056</v>
+      </c>
+      <c r="M28">
+        <v>1121</v>
+      </c>
+      <c r="N28">
+        <f>LOG(J28)</f>
+        <v>5.237531171569807</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="0"/>
+        <v>5.3710678622717358</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="0"/>
+        <v>5.2331383122024064</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="0"/>
+        <v>3.0496056125949731</v>
+      </c>
+    </row>
+    <row r="29" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>100000</v>
+      </c>
+      <c r="J29">
+        <v>2091718</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>2350000</v>
+      </c>
+      <c r="L29">
+        <v>1641879</v>
+      </c>
+      <c r="M29">
+        <v>18221</v>
+      </c>
+      <c r="N29">
+        <f>LOG(J29)</f>
+        <v>6.3205031336851318</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="0"/>
+        <v>6.3710678622717358</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="0"/>
+        <v>6.2153411481740353</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="0"/>
+        <v>4.2605722081234925</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add % speedup + medians
</commit_message>
<xml_diff>
--- a/PerformanceGraphs.xlsx
+++ b/PerformanceGraphs.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3105" yWindow="0" windowWidth="20505" windowHeight="9120" activeTab="1"/>
+    <workbookView xWindow="4140" yWindow="0" windowWidth="20505" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="ReadTests" sheetId="1" r:id="rId1"/>
     <sheet name="WriteTests" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>Count</t>
   </si>
@@ -62,6 +63,18 @@
   <si>
     <t>* Time is in milliseconds</t>
   </si>
+  <si>
+    <t>PerItem Simple</t>
+  </si>
+  <si>
+    <t>PerItem Expected</t>
+  </si>
+  <si>
+    <t>PerItem Parallel</t>
+  </si>
+  <si>
+    <t>PerItem Bulk</t>
+  </si>
 </sst>
 </file>
 
@@ -96,8 +109,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,11 +461,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="241015312"/>
-        <c:axId val="241012960"/>
+        <c:axId val="324569376"/>
+        <c:axId val="324572120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="241015312"/>
+        <c:axId val="324569376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,7 +508,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241012960"/>
+        <c:crossAx val="324572120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -502,7 +516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241012960"/>
+        <c:axId val="324572120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,7 +567,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241015312"/>
+        <c:crossAx val="324569376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -966,11 +980,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="286410128"/>
-        <c:axId val="240764272"/>
+        <c:axId val="324570944"/>
+        <c:axId val="324567024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="286410128"/>
+        <c:axId val="324570944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1013,7 +1027,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240764272"/>
+        <c:crossAx val="324567024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1021,7 +1035,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="240764272"/>
+        <c:axId val="324567024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1072,7 +1086,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286410128"/>
+        <c:crossAx val="324570944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2600,10 +2614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="I20:Q29"/>
+  <dimension ref="I20:U31"/>
   <sheetViews>
-    <sheetView topLeftCell="K3" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="N9" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2615,9 +2629,13 @@
     <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="20" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I20" t="s">
         <v>9</v>
       </c>
@@ -2625,12 +2643,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
         <v>0</v>
       </c>
@@ -2658,8 +2676,20 @@
       <c r="Q23" t="s">
         <v>8</v>
       </c>
+      <c r="R23" t="s">
+        <v>12</v>
+      </c>
+      <c r="S23" t="s">
+        <v>13</v>
+      </c>
+      <c r="T23" t="s">
+        <v>14</v>
+      </c>
+      <c r="U23" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="24" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I24">
         <v>1</v>
       </c>
@@ -2691,8 +2721,24 @@
         <f>LOG(M24)</f>
         <v>1.0791812460476249</v>
       </c>
+      <c r="R24">
+        <f>J24/$I24</f>
+        <v>10</v>
+      </c>
+      <c r="S24">
+        <f t="shared" ref="S24:U29" si="0">K24/$I24</f>
+        <v>2.1</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
     </row>
-    <row r="25" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I25">
         <v>10</v>
       </c>
@@ -2713,19 +2759,35 @@
         <v>1.3222192947339193</v>
       </c>
       <c r="O25">
-        <f t="shared" ref="O25:O29" si="0">LOG(K25)</f>
+        <f t="shared" ref="O25:O29" si="1">LOG(K25)</f>
         <v>1.3222192947339193</v>
       </c>
       <c r="P25">
-        <f t="shared" ref="P25:P29" si="1">LOG(L25)</f>
+        <f t="shared" ref="P25:P29" si="2">LOG(L25)</f>
         <v>1.2787536009528289</v>
       </c>
       <c r="Q25">
-        <f t="shared" ref="Q25:Q29" si="2">LOG(M25)</f>
+        <f t="shared" ref="Q25:Q29" si="3">LOG(M25)</f>
         <v>0</v>
       </c>
+      <c r="R25">
+        <f t="shared" ref="R25:R29" si="4">J25/$I25</f>
+        <v>2.1</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="26" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I26">
         <v>100</v>
       </c>
@@ -2747,19 +2809,35 @@
         <v>1.9294189257142926</v>
       </c>
       <c r="O26">
+        <f t="shared" si="1"/>
+        <v>2.3222192947339191</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="2"/>
+        <v>1.7781512503836436</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="4"/>
+        <v>0.85</v>
+      </c>
+      <c r="S26">
         <f t="shared" si="0"/>
-        <v>2.3222192947339191</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="1"/>
-        <v>1.7781512503836436</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2.1</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I27">
         <v>1000</v>
       </c>
@@ -2781,19 +2859,35 @@
         <v>2.9079485216122722</v>
       </c>
       <c r="O27">
+        <f t="shared" si="1"/>
+        <v>3.3222192947339191</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="2"/>
+        <v>2.4983105537896004</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="3"/>
+        <v>1.9777236052888478</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="4"/>
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="S27">
         <f t="shared" si="0"/>
-        <v>3.3222192947339191</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="1"/>
-        <v>2.4983105537896004</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="2"/>
-        <v>1.9777236052888478</v>
+        <v>2.1</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="0"/>
+        <v>0.315</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="0"/>
+        <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I28">
         <v>10000</v>
       </c>
@@ -2801,7 +2895,7 @@
         <v>6691</v>
       </c>
       <c r="K28">
-        <f t="shared" ref="K28:K29" si="3">K27*10</f>
+        <f t="shared" ref="K28:K29" si="5">K27*10</f>
         <v>21000</v>
       </c>
       <c r="L28">
@@ -2815,19 +2909,35 @@
         <v>3.8254910298794309</v>
       </c>
       <c r="O28">
+        <f t="shared" si="1"/>
+        <v>4.3222192947339195</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="2"/>
+        <v>3.4795753101749884</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="3"/>
+        <v>2.9800033715837464</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="4"/>
+        <v>0.66910000000000003</v>
+      </c>
+      <c r="S28">
         <f t="shared" si="0"/>
-        <v>4.3222192947339195</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="1"/>
-        <v>3.4795753101749884</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="2"/>
-        <v>2.9800033715837464</v>
+        <v>2.1</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="0"/>
+        <v>0.30170000000000002</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="0"/>
+        <v>9.5500000000000002E-2</v>
       </c>
     </row>
-    <row r="29" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I29">
         <v>100000</v>
       </c>
@@ -2835,7 +2945,7 @@
         <v>61620</v>
       </c>
       <c r="K29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>210000</v>
       </c>
       <c r="L29">
@@ -2849,16 +2959,60 @@
         <v>4.7897216939809217</v>
       </c>
       <c r="O29">
+        <f t="shared" si="1"/>
+        <v>5.3222192947339195</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="2"/>
+        <v>4.3745650607227651</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="3"/>
+        <v>3.9711366294768062</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="4"/>
+        <v>0.61619999999999997</v>
+      </c>
+      <c r="S29">
         <f t="shared" si="0"/>
-        <v>5.3222192947339195</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="1"/>
-        <v>4.3745650607227651</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="2"/>
-        <v>3.9711366294768062</v>
+        <v>2.1</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="0"/>
+        <v>0.2369</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="0"/>
+        <v>9.357E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="R30">
+        <f>MEDIAN(R24:R29)</f>
+        <v>0.82950000000000002</v>
+      </c>
+      <c r="S30">
+        <f t="shared" ref="S30:U30" si="6">MEDIAN(S24:S29)</f>
+        <v>2.1</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="6"/>
+        <v>0.45750000000000002</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="6"/>
+        <v>9.7750000000000004E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="T31">
+        <f>R30/T30</f>
+        <v>1.8131147540983605</v>
+      </c>
+      <c r="U31">
+        <f>S30/U30</f>
+        <v>21.483375959079282</v>
       </c>
     </row>
   </sheetData>
@@ -2869,10 +3023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="I20:Q29"/>
+  <dimension ref="I20:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L4" workbookViewId="0">
-      <selection activeCell="O30" sqref="O30"/>
+    <sheetView topLeftCell="I10" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2884,9 +3038,13 @@
     <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="20" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I20" t="s">
         <v>9</v>
       </c>
@@ -2894,12 +3052,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
         <v>0</v>
       </c>
@@ -2927,8 +3085,20 @@
       <c r="Q23" t="s">
         <v>8</v>
       </c>
+      <c r="R23" t="s">
+        <v>12</v>
+      </c>
+      <c r="S23" t="s">
+        <v>13</v>
+      </c>
+      <c r="T23" t="s">
+        <v>14</v>
+      </c>
+      <c r="U23" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="24" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I24">
         <v>1</v>
       </c>
@@ -2960,8 +3130,24 @@
         <f>LOG(M24)</f>
         <v>2.4297522800024081</v>
       </c>
+      <c r="R24" s="1">
+        <f>J24/$I24</f>
+        <v>411</v>
+      </c>
+      <c r="S24" s="1">
+        <f t="shared" ref="S24:U24" si="0">K24/$I24</f>
+        <v>2.1</v>
+      </c>
+      <c r="T24" s="1">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="U24" s="1">
+        <f t="shared" si="0"/>
+        <v>269</v>
+      </c>
     </row>
-    <row r="25" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I25">
         <v>10</v>
       </c>
@@ -2982,19 +3168,35 @@
         <v>2.3710678622717363</v>
       </c>
       <c r="O25">
-        <f t="shared" ref="O25:Q29" si="0">LOG(K25)</f>
+        <f t="shared" ref="O25:Q29" si="1">LOG(K25)</f>
         <v>1.3222192947339193</v>
       </c>
       <c r="P25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.271841606536499</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4313637641589874</v>
       </c>
+      <c r="R25" s="1">
+        <f t="shared" ref="R25:R29" si="2">J25/I25</f>
+        <v>23.5</v>
+      </c>
+      <c r="S25" s="1">
+        <f t="shared" ref="S25:S29" si="3">K25/$I25</f>
+        <v>2.1</v>
+      </c>
+      <c r="T25" s="1">
+        <f t="shared" ref="T25:T29" si="4">L25/$I25</f>
+        <v>18.7</v>
+      </c>
+      <c r="U25" s="1">
+        <f t="shared" ref="U25:U29" si="5">M25/$I25</f>
+        <v>2.7</v>
+      </c>
     </row>
-    <row r="26" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I26">
         <v>100</v>
       </c>
@@ -3016,19 +3218,35 @@
         <v>3.1989318699322089</v>
       </c>
       <c r="O26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.3710678622717363</v>
       </c>
       <c r="P26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1983821300082944</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2304489213782739</v>
       </c>
+      <c r="R26" s="1">
+        <f t="shared" si="2"/>
+        <v>15.81</v>
+      </c>
+      <c r="S26" s="1">
+        <f t="shared" si="3"/>
+        <v>23.5</v>
+      </c>
+      <c r="T26" s="1">
+        <f t="shared" si="4"/>
+        <v>15.79</v>
+      </c>
+      <c r="U26" s="1">
+        <f t="shared" si="5"/>
+        <v>0.17</v>
+      </c>
     </row>
-    <row r="27" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I27">
         <v>1000</v>
       </c>
@@ -3050,19 +3268,35 @@
         <v>4.295083059251656</v>
       </c>
       <c r="O27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.3710678622717358</v>
       </c>
       <c r="P27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.224895470849483</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7853298350107671</v>
       </c>
+      <c r="R27" s="1">
+        <f t="shared" si="2"/>
+        <v>19.728000000000002</v>
+      </c>
+      <c r="S27" s="1">
+        <f t="shared" si="3"/>
+        <v>23.5</v>
+      </c>
+      <c r="T27" s="1">
+        <f t="shared" si="4"/>
+        <v>16.783999999999999</v>
+      </c>
+      <c r="U27" s="1">
+        <f t="shared" si="5"/>
+        <v>6.0999999999999999E-2</v>
+      </c>
     </row>
-    <row r="28" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I28">
         <v>10000</v>
       </c>
@@ -3070,7 +3304,7 @@
         <v>172795</v>
       </c>
       <c r="K28">
-        <f t="shared" ref="K28:K29" si="1">K27*10</f>
+        <f t="shared" ref="K28:K29" si="6">K27*10</f>
         <v>235000</v>
       </c>
       <c r="L28">
@@ -3084,19 +3318,35 @@
         <v>5.237531171569807</v>
       </c>
       <c r="O28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.3710678622717358</v>
       </c>
       <c r="P28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.2331383122024064</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.0496056125949731</v>
       </c>
+      <c r="R28" s="1">
+        <f t="shared" si="2"/>
+        <v>17.279499999999999</v>
+      </c>
+      <c r="S28" s="1">
+        <f t="shared" si="3"/>
+        <v>23.5</v>
+      </c>
+      <c r="T28" s="1">
+        <f t="shared" si="4"/>
+        <v>17.105599999999999</v>
+      </c>
+      <c r="U28" s="1">
+        <f t="shared" si="5"/>
+        <v>0.11210000000000001</v>
+      </c>
     </row>
-    <row r="29" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:21" x14ac:dyDescent="0.25">
       <c r="I29">
         <v>100000</v>
       </c>
@@ -3104,7 +3354,7 @@
         <v>2091718</v>
       </c>
       <c r="K29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>2350000</v>
       </c>
       <c r="L29">
@@ -3118,20 +3368,65 @@
         <v>6.3205031336851318</v>
       </c>
       <c r="O29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.3710678622717358</v>
       </c>
       <c r="P29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.2153411481740353</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.2605722081234925</v>
+      </c>
+      <c r="R29" s="1">
+        <f t="shared" si="2"/>
+        <v>20.917179999999998</v>
+      </c>
+      <c r="S29" s="1">
+        <f t="shared" si="3"/>
+        <v>23.5</v>
+      </c>
+      <c r="T29" s="1">
+        <f t="shared" si="4"/>
+        <v>16.418790000000001</v>
+      </c>
+      <c r="U29" s="1">
+        <f t="shared" si="5"/>
+        <v>0.18221000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="R30" s="1">
+        <f>MEDIAN(R24:R29)</f>
+        <v>20.322589999999998</v>
+      </c>
+      <c r="S30" s="1">
+        <f t="shared" ref="S30:U30" si="7">MEDIAN(S24:S29)</f>
+        <v>23.5</v>
+      </c>
+      <c r="T30" s="1">
+        <f t="shared" si="7"/>
+        <v>16.944800000000001</v>
+      </c>
+      <c r="U30" s="1">
+        <f t="shared" si="7"/>
+        <v>0.17610500000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="T31" s="1">
+        <f>$R$30/T30</f>
+        <v>1.1993408007176241</v>
+      </c>
+      <c r="U31" s="1">
+        <f>$R$30/U30</f>
+        <v>115.40041452542515</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update graphs to include SQLCE
</commit_message>
<xml_diff>
--- a/PerformanceGraphs.xlsx
+++ b/PerformanceGraphs.xlsx
@@ -9,14 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="0" windowWidth="20505" windowHeight="9120"/>
+    <workbookView xWindow="5175" yWindow="0" windowWidth="20505" windowHeight="9120"/>
   </bookViews>
   <sheets>
     <sheet name="ReadTests" sheetId="1" r:id="rId1"/>
     <sheet name="WriteTests" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>Count</t>
   </si>
@@ -74,6 +73,33 @@
   </si>
   <si>
     <t>PerItem Bulk</t>
+  </si>
+  <si>
+    <t>SQLCE Simple</t>
+  </si>
+  <si>
+    <t>Log(SQLCE Simple)</t>
+  </si>
+  <si>
+    <t>PerItem SQLCE Simple</t>
+  </si>
+  <si>
+    <t>SQLCE Parallel</t>
+  </si>
+  <si>
+    <t>SQLCE Bulk</t>
+  </si>
+  <si>
+    <t>Log(SQLCE Parallel)</t>
+  </si>
+  <si>
+    <t>Log(SQLCE Bulk)</t>
+  </si>
+  <si>
+    <t>PerItem SQLCE Parallel</t>
+  </si>
+  <si>
+    <t>PerItem SQLCE Bulk</t>
   </si>
 </sst>
 </file>
@@ -210,7 +236,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>ReadTests!$N$23</c:f>
+              <c:f>ReadTests!$Q$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -260,7 +286,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ReadTests!$N$24:$N$29</c:f>
+              <c:f>ReadTests!$Q$24:$Q$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -292,7 +318,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>ReadTests!$O$23</c:f>
+              <c:f>ReadTests!$R$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -315,7 +341,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>ReadTests!$O$24:$O$29</c:f>
+              <c:f>ReadTests!$R$24:$R$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -347,7 +373,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>ReadTests!$P$23</c:f>
+              <c:f>ReadTests!$S$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -370,7 +396,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>ReadTests!$P$24:$P$29</c:f>
+              <c:f>ReadTests!$S$24:$S$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -402,7 +428,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>ReadTests!$Q$23</c:f>
+              <c:f>ReadTests!$T$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -425,7 +451,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>ReadTests!$Q$24:$Q$29</c:f>
+              <c:f>ReadTests!$T$24:$T$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -446,6 +472,116 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.9711366294768062</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ReadTests!$U$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Log(SQLCE Simple)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>ReadTests!$U$24:$U$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.3010299956639812</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90308998699194354</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9395192526186185</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7958800173440754</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8874485002499535</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.8823822163144444</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ReadTests!$V$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Log(SQLCE Parallel)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>ReadTests!$V$24:$V$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.3617278360175928</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77815125038364363</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7781512503836436</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9542425094393248</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.8882918453565156</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9125196349870226</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,11 +597,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="324569376"/>
-        <c:axId val="324572120"/>
+        <c:axId val="320964096"/>
+        <c:axId val="320964488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="324569376"/>
+        <c:axId val="320964096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,7 +644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324572120"/>
+        <c:crossAx val="320964488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -516,7 +652,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324572120"/>
+        <c:axId val="320964488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,7 +703,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324569376"/>
+        <c:crossAx val="320964096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -729,7 +865,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>WriteTests!$N$23</c:f>
+              <c:f>WriteTests!$Q$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -779,7 +915,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>WriteTests!$N$24:$N$29</c:f>
+              <c:f>WriteTests!$Q$24:$Q$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -811,7 +947,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>WriteTests!$O$23</c:f>
+              <c:f>WriteTests!$R$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -834,7 +970,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>WriteTests!$O$24:$O$29</c:f>
+              <c:f>WriteTests!$R$24:$R$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -866,7 +1002,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>WriteTests!$P$23</c:f>
+              <c:f>WriteTests!$S$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -889,7 +1025,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>WriteTests!$P$24:$P$29</c:f>
+              <c:f>WriteTests!$S$24:$S$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -921,7 +1057,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>WriteTests!$Q$23</c:f>
+              <c:f>WriteTests!$T$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -944,7 +1080,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>WriteTests!$Q$24:$Q$29</c:f>
+              <c:f>WriteTests!$T$24:$T$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -965,6 +1101,173 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.2605722081234925</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>WriteTests!$U$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Log(SQLCE Simple)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>WriteTests!$U$24:$U$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.1818435879447726</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.146128035678238</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2278867046136734</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2898118391176214</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0280422950907493</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1510387162491984</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>WriteTests!$V$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Log(SQLCE Parallel)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>WriteTests!$V$24:$V$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.1643528557844371</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1139433523068367</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2380461031287955</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1179338350396413</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9887372752888002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0546819847184326</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>WriteTests!$W$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Log(SQLCE Bulk)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>WriteTests!$W$24:$W$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.255272505103306</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3222192947339193</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0718820073061255</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1215598441875008</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.009748255948554</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0726799340352233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -980,11 +1283,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="324570944"/>
-        <c:axId val="324567024"/>
+        <c:axId val="320960176"/>
+        <c:axId val="320961352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="324570944"/>
+        <c:axId val="320960176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1027,7 +1330,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324567024"/>
+        <c:crossAx val="320961352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1035,7 +1338,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324567024"/>
+        <c:axId val="320961352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1086,7 +1389,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324570944"/>
+        <c:crossAx val="320960176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2289,8 +2592,8 @@
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>538162</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -2324,8 +2627,8 @@
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>538162</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -2614,10 +2917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="I20:U31"/>
+  <dimension ref="I20:AD31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N9" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" topLeftCell="L5" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2625,30 +2928,36 @@
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="15.85546875" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="15.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="20" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I20" t="s">
         <v>9</v>
       </c>
-      <c r="P20" t="s">
+      <c r="S20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
         <v>0</v>
       </c>
@@ -2665,31 +2974,58 @@
         <v>7</v>
       </c>
       <c r="N23" t="s">
+        <v>16</v>
+      </c>
+      <c r="O23" t="s">
+        <v>19</v>
+      </c>
+      <c r="P23" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q23" t="s">
         <v>4</v>
       </c>
-      <c r="O23" t="s">
+      <c r="R23" t="s">
         <v>1</v>
       </c>
-      <c r="P23" t="s">
+      <c r="S23" t="s">
         <v>5</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="T23" t="s">
         <v>8</v>
       </c>
-      <c r="R23" t="s">
+      <c r="U23" t="s">
+        <v>17</v>
+      </c>
+      <c r="V23" t="s">
+        <v>21</v>
+      </c>
+      <c r="W23" t="s">
+        <v>22</v>
+      </c>
+      <c r="X23" t="s">
         <v>12</v>
       </c>
-      <c r="S23" t="s">
+      <c r="Y23" t="s">
         <v>13</v>
       </c>
-      <c r="T23" t="s">
+      <c r="Z23" t="s">
         <v>14</v>
       </c>
-      <c r="U23" t="s">
+      <c r="AA23" t="s">
         <v>15</v>
       </c>
+      <c r="AB23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="24" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I24">
         <v>1</v>
       </c>
@@ -2706,39 +3042,72 @@
         <v>12</v>
       </c>
       <c r="N24">
+        <v>2</v>
+      </c>
+      <c r="O24">
+        <v>23</v>
+      </c>
+      <c r="P24">
+        <v>27</v>
+      </c>
+      <c r="Q24">
         <f>LOG(J24)</f>
         <v>1</v>
       </c>
-      <c r="O24">
+      <c r="R24">
         <f>LOG(K24)</f>
         <v>0.3222192947339193</v>
       </c>
-      <c r="P24">
+      <c r="S24">
         <f>LOG(L24)</f>
         <v>1.5440680443502757</v>
       </c>
-      <c r="Q24">
+      <c r="T24">
         <f>LOG(M24)</f>
         <v>1.0791812460476249</v>
       </c>
-      <c r="R24">
+      <c r="U24">
+        <f>LOG(N24)</f>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="V24">
+        <f t="shared" ref="V24:W24" si="0">LOG(O24)</f>
+        <v>1.3617278360175928</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="0"/>
+        <v>1.4313637641589874</v>
+      </c>
+      <c r="X24">
         <f>J24/$I24</f>
         <v>10</v>
       </c>
-      <c r="S24">
-        <f t="shared" ref="S24:U29" si="0">K24/$I24</f>
+      <c r="Y24">
+        <f>K24/$I24</f>
         <v>2.1</v>
       </c>
-      <c r="T24">
-        <f t="shared" si="0"/>
+      <c r="Z24">
+        <f>L24/$I24</f>
         <v>35</v>
       </c>
-      <c r="U24">
-        <f t="shared" si="0"/>
+      <c r="AA24">
+        <f>M24/$I24</f>
         <v>12</v>
       </c>
+      <c r="AB24">
+        <f>N24/$I24</f>
+        <v>2</v>
+      </c>
+      <c r="AC24">
+        <f t="shared" ref="AC24:AD24" si="1">O24/$I24</f>
+        <v>23</v>
+      </c>
+      <c r="AD24">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
     </row>
-    <row r="25" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I25">
         <v>10</v>
       </c>
@@ -2755,39 +3124,72 @@
         <v>1</v>
       </c>
       <c r="N25">
+        <v>8</v>
+      </c>
+      <c r="O25">
+        <v>6</v>
+      </c>
+      <c r="P25">
+        <v>2</v>
+      </c>
+      <c r="Q25">
         <f>LOG(J25)</f>
         <v>1.3222192947339193</v>
       </c>
-      <c r="O25">
-        <f t="shared" ref="O25:O29" si="1">LOG(K25)</f>
+      <c r="R25">
+        <f>LOG(K25)</f>
         <v>1.3222192947339193</v>
       </c>
-      <c r="P25">
-        <f t="shared" ref="P25:P29" si="2">LOG(L25)</f>
+      <c r="S25">
+        <f>LOG(L25)</f>
         <v>1.2787536009528289</v>
       </c>
-      <c r="Q25">
-        <f t="shared" ref="Q25:Q29" si="3">LOG(M25)</f>
+      <c r="T25">
+        <f>LOG(M25)</f>
         <v>0</v>
       </c>
-      <c r="R25">
-        <f t="shared" ref="R25:R29" si="4">J25/$I25</f>
+      <c r="U25">
+        <f t="shared" ref="U25:U29" si="2">LOG(N25)</f>
+        <v>0.90308998699194354</v>
+      </c>
+      <c r="V25">
+        <f t="shared" ref="V25:V29" si="3">LOG(O25)</f>
+        <v>0.77815125038364363</v>
+      </c>
+      <c r="W25">
+        <f t="shared" ref="W25:W29" si="4">LOG(P25)</f>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="X25">
+        <f>J25/$I25</f>
         <v>2.1</v>
       </c>
-      <c r="S25">
-        <f t="shared" si="0"/>
+      <c r="Y25">
+        <f>K25/$I25</f>
         <v>2.1</v>
       </c>
-      <c r="T25">
-        <f t="shared" si="0"/>
+      <c r="Z25">
+        <f>L25/$I25</f>
         <v>1.9</v>
       </c>
-      <c r="U25">
-        <f t="shared" si="0"/>
+      <c r="AA25">
+        <f>M25/$I25</f>
         <v>0.1</v>
       </c>
+      <c r="AB25">
+        <f t="shared" ref="AB25:AB30" si="5">N25/$I25</f>
+        <v>0.8</v>
+      </c>
+      <c r="AC25">
+        <f t="shared" ref="AC25:AC30" si="6">O25/$I25</f>
+        <v>0.6</v>
+      </c>
+      <c r="AD25">
+        <f t="shared" ref="AD25:AD30" si="7">P25/$I25</f>
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="26" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I26">
         <v>100</v>
       </c>
@@ -2805,39 +3207,72 @@
         <v>10</v>
       </c>
       <c r="N26">
+        <v>87</v>
+      </c>
+      <c r="O26">
+        <v>60</v>
+      </c>
+      <c r="P26">
+        <v>37</v>
+      </c>
+      <c r="Q26">
         <f>LOG(J26)</f>
         <v>1.9294189257142926</v>
       </c>
-      <c r="O26">
-        <f t="shared" si="1"/>
+      <c r="R26">
+        <f>LOG(K26)</f>
         <v>2.3222192947339191</v>
       </c>
-      <c r="P26">
+      <c r="S26">
+        <f>LOG(L26)</f>
+        <v>1.7781512503836436</v>
+      </c>
+      <c r="T26">
+        <f>LOG(M26)</f>
+        <v>1</v>
+      </c>
+      <c r="U26">
         <f t="shared" si="2"/>
+        <v>1.9395192526186185</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="3"/>
         <v>1.7781512503836436</v>
       </c>
-      <c r="Q26">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="R26">
+      <c r="W26">
         <f t="shared" si="4"/>
+        <v>1.568201724066995</v>
+      </c>
+      <c r="X26">
+        <f>J26/$I26</f>
         <v>0.85</v>
       </c>
-      <c r="S26">
-        <f t="shared" si="0"/>
+      <c r="Y26">
+        <f>K26/$I26</f>
         <v>2.1</v>
       </c>
-      <c r="T26">
-        <f t="shared" si="0"/>
+      <c r="Z26">
+        <f>L26/$I26</f>
         <v>0.6</v>
       </c>
-      <c r="U26">
-        <f t="shared" si="0"/>
+      <c r="AA26">
+        <f>M26/$I26</f>
         <v>0.1</v>
       </c>
+      <c r="AB26">
+        <f t="shared" si="5"/>
+        <v>0.87</v>
+      </c>
+      <c r="AC26">
+        <f t="shared" si="6"/>
+        <v>0.6</v>
+      </c>
+      <c r="AD26">
+        <f t="shared" si="7"/>
+        <v>0.37</v>
+      </c>
     </row>
-    <row r="27" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I27">
         <v>1000</v>
       </c>
@@ -2855,39 +3290,72 @@
         <v>95</v>
       </c>
       <c r="N27">
+        <v>625</v>
+      </c>
+      <c r="O27">
+        <v>900</v>
+      </c>
+      <c r="P27">
+        <v>372</v>
+      </c>
+      <c r="Q27">
         <f>LOG(J27)</f>
         <v>2.9079485216122722</v>
       </c>
-      <c r="O27">
-        <f t="shared" si="1"/>
+      <c r="R27">
+        <f>LOG(K27)</f>
         <v>3.3222192947339191</v>
       </c>
-      <c r="P27">
+      <c r="S27">
+        <f>LOG(L27)</f>
+        <v>2.4983105537896004</v>
+      </c>
+      <c r="T27">
+        <f>LOG(M27)</f>
+        <v>1.9777236052888478</v>
+      </c>
+      <c r="U27">
         <f t="shared" si="2"/>
-        <v>2.4983105537896004</v>
-      </c>
-      <c r="Q27">
+        <v>2.7958800173440754</v>
+      </c>
+      <c r="V27">
         <f t="shared" si="3"/>
-        <v>1.9777236052888478</v>
-      </c>
-      <c r="R27">
+        <v>2.9542425094393248</v>
+      </c>
+      <c r="W27">
         <f t="shared" si="4"/>
+        <v>2.5705429398818973</v>
+      </c>
+      <c r="X27">
+        <f>J27/$I27</f>
         <v>0.80900000000000005</v>
       </c>
-      <c r="S27">
-        <f t="shared" si="0"/>
+      <c r="Y27">
+        <f>K27/$I27</f>
         <v>2.1</v>
       </c>
-      <c r="T27">
-        <f t="shared" si="0"/>
+      <c r="Z27">
+        <f>L27/$I27</f>
         <v>0.315</v>
       </c>
-      <c r="U27">
-        <f t="shared" si="0"/>
+      <c r="AA27">
+        <f>M27/$I27</f>
         <v>9.5000000000000001E-2</v>
       </c>
+      <c r="AB27">
+        <f t="shared" si="5"/>
+        <v>0.625</v>
+      </c>
+      <c r="AC27">
+        <f t="shared" si="6"/>
+        <v>0.9</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="7"/>
+        <v>0.372</v>
+      </c>
     </row>
-    <row r="28" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I28">
         <v>10000</v>
       </c>
@@ -2895,7 +3363,7 @@
         <v>6691</v>
       </c>
       <c r="K28">
-        <f t="shared" ref="K28:K29" si="5">K27*10</f>
+        <f t="shared" ref="K28:K29" si="8">K27*10</f>
         <v>21000</v>
       </c>
       <c r="L28">
@@ -2905,39 +3373,72 @@
         <v>955</v>
       </c>
       <c r="N28">
+        <v>7717</v>
+      </c>
+      <c r="O28">
+        <v>7732</v>
+      </c>
+      <c r="P28">
+        <v>2573</v>
+      </c>
+      <c r="Q28">
         <f>LOG(J28)</f>
         <v>3.8254910298794309</v>
       </c>
-      <c r="O28">
-        <f t="shared" si="1"/>
+      <c r="R28">
+        <f>LOG(K28)</f>
         <v>4.3222192947339195</v>
       </c>
-      <c r="P28">
+      <c r="S28">
+        <f>LOG(L28)</f>
+        <v>3.4795753101749884</v>
+      </c>
+      <c r="T28">
+        <f>LOG(M28)</f>
+        <v>2.9800033715837464</v>
+      </c>
+      <c r="U28">
         <f t="shared" si="2"/>
-        <v>3.4795753101749884</v>
-      </c>
-      <c r="Q28">
+        <v>3.8874485002499535</v>
+      </c>
+      <c r="V28">
         <f t="shared" si="3"/>
-        <v>2.9800033715837464</v>
-      </c>
-      <c r="R28">
+        <v>3.8882918453565156</v>
+      </c>
+      <c r="W28">
         <f t="shared" si="4"/>
+        <v>3.4104397862103464</v>
+      </c>
+      <c r="X28">
+        <f>J28/$I28</f>
         <v>0.66910000000000003</v>
       </c>
-      <c r="S28">
-        <f t="shared" si="0"/>
+      <c r="Y28">
+        <f>K28/$I28</f>
         <v>2.1</v>
       </c>
-      <c r="T28">
-        <f t="shared" si="0"/>
+      <c r="Z28">
+        <f>L28/$I28</f>
         <v>0.30170000000000002</v>
       </c>
-      <c r="U28">
-        <f t="shared" si="0"/>
+      <c r="AA28">
+        <f>M28/$I28</f>
         <v>9.5500000000000002E-2</v>
       </c>
+      <c r="AB28">
+        <f t="shared" si="5"/>
+        <v>0.77170000000000005</v>
+      </c>
+      <c r="AC28">
+        <f t="shared" si="6"/>
+        <v>0.7732</v>
+      </c>
+      <c r="AD28">
+        <f t="shared" si="7"/>
+        <v>0.25729999999999997</v>
+      </c>
     </row>
-    <row r="29" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I29">
         <v>100000</v>
       </c>
@@ -2945,7 +3446,7 @@
         <v>61620</v>
       </c>
       <c r="K29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>210000</v>
       </c>
       <c r="L29">
@@ -2955,64 +3456,121 @@
         <v>9357</v>
       </c>
       <c r="N29">
+        <v>76275</v>
+      </c>
+      <c r="O29">
+        <v>81756</v>
+      </c>
+      <c r="P29">
+        <v>22503</v>
+      </c>
+      <c r="Q29">
         <f>LOG(J29)</f>
         <v>4.7897216939809217</v>
       </c>
-      <c r="O29">
-        <f t="shared" si="1"/>
+      <c r="R29">
+        <f>LOG(K29)</f>
         <v>5.3222192947339195</v>
       </c>
-      <c r="P29">
+      <c r="S29">
+        <f>LOG(L29)</f>
+        <v>4.3745650607227651</v>
+      </c>
+      <c r="T29">
+        <f>LOG(M29)</f>
+        <v>3.9711366294768062</v>
+      </c>
+      <c r="U29">
         <f t="shared" si="2"/>
-        <v>4.3745650607227651</v>
-      </c>
-      <c r="Q29">
+        <v>4.8823822163144444</v>
+      </c>
+      <c r="V29">
         <f t="shared" si="3"/>
-        <v>3.9711366294768062</v>
-      </c>
-      <c r="R29">
+        <v>4.9125196349870226</v>
+      </c>
+      <c r="W29">
         <f t="shared" si="4"/>
+        <v>4.3522404201822305</v>
+      </c>
+      <c r="X29">
+        <f>J29/$I29</f>
         <v>0.61619999999999997</v>
       </c>
-      <c r="S29">
-        <f t="shared" si="0"/>
+      <c r="Y29">
+        <f>K29/$I29</f>
         <v>2.1</v>
       </c>
-      <c r="T29">
-        <f t="shared" si="0"/>
+      <c r="Z29">
+        <f>L29/$I29</f>
         <v>0.2369</v>
       </c>
-      <c r="U29">
-        <f t="shared" si="0"/>
+      <c r="AA29">
+        <f>M29/$I29</f>
         <v>9.357E-2</v>
       </c>
+      <c r="AB29">
+        <f t="shared" si="5"/>
+        <v>0.76275000000000004</v>
+      </c>
+      <c r="AC29">
+        <f t="shared" si="6"/>
+        <v>0.81755999999999995</v>
+      </c>
+      <c r="AD29">
+        <f t="shared" si="7"/>
+        <v>0.22503000000000001</v>
+      </c>
     </row>
-    <row r="30" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="R30">
-        <f>MEDIAN(R24:R29)</f>
+    <row r="30" spans="9:30" x14ac:dyDescent="0.25">
+      <c r="X30">
+        <f>MEDIAN(X24:X29)</f>
         <v>0.82950000000000002</v>
       </c>
-      <c r="S30">
-        <f t="shared" ref="S30:U30" si="6">MEDIAN(S24:S29)</f>
+      <c r="Y30">
+        <f t="shared" ref="Y30:AD30" si="9">MEDIAN(Y24:Y29)</f>
         <v>2.1</v>
       </c>
-      <c r="T30">
-        <f t="shared" si="6"/>
+      <c r="Z30">
+        <f t="shared" si="9"/>
         <v>0.45750000000000002</v>
       </c>
-      <c r="U30">
-        <f t="shared" si="6"/>
+      <c r="AA30">
+        <f t="shared" si="9"/>
         <v>9.7750000000000004E-2</v>
       </c>
+      <c r="AB30">
+        <f t="shared" si="9"/>
+        <v>0.78585000000000005</v>
+      </c>
+      <c r="AC30">
+        <f t="shared" si="9"/>
+        <v>0.79537999999999998</v>
+      </c>
+      <c r="AD30">
+        <f t="shared" si="9"/>
+        <v>0.31364999999999998</v>
+      </c>
     </row>
-    <row r="31" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="T31">
-        <f>R30/T30</f>
+    <row r="31" spans="9:30" x14ac:dyDescent="0.25">
+      <c r="Z31">
+        <f>X30/Z30</f>
         <v>1.8131147540983605</v>
       </c>
-      <c r="U31">
-        <f>S30/U30</f>
+      <c r="AA31">
+        <f>Y30/AA30</f>
         <v>21.483375959079282</v>
+      </c>
+      <c r="AB31">
+        <f t="shared" ref="AB31:AD31" si="10">Z30/AB30</f>
+        <v>0.58217217026150025</v>
+      </c>
+      <c r="AC31">
+        <f t="shared" si="10"/>
+        <v>0.1228972315119817</v>
+      </c>
+      <c r="AD31">
+        <f t="shared" si="10"/>
+        <v>2.5054997608799621</v>
       </c>
     </row>
   </sheetData>
@@ -3023,10 +3581,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="I20:U31"/>
+  <dimension ref="I20:AD31"/>
   <sheetViews>
-    <sheetView topLeftCell="I10" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView topLeftCell="M10" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3034,30 +3592,33 @@
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="15.85546875" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="16" width="15.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="17.7109375" customWidth="1"/>
+    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="20" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I20" t="s">
         <v>9</v>
       </c>
-      <c r="P20" t="s">
+      <c r="S20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
         <v>0</v>
       </c>
@@ -3074,31 +3635,58 @@
         <v>7</v>
       </c>
       <c r="N23" t="s">
+        <v>16</v>
+      </c>
+      <c r="O23" t="s">
+        <v>19</v>
+      </c>
+      <c r="P23" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q23" t="s">
         <v>4</v>
       </c>
-      <c r="O23" t="s">
+      <c r="R23" t="s">
         <v>1</v>
       </c>
-      <c r="P23" t="s">
+      <c r="S23" t="s">
         <v>5</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="T23" t="s">
         <v>8</v>
       </c>
-      <c r="R23" t="s">
+      <c r="U23" t="s">
+        <v>17</v>
+      </c>
+      <c r="V23" t="s">
+        <v>21</v>
+      </c>
+      <c r="W23" t="s">
+        <v>22</v>
+      </c>
+      <c r="X23" t="s">
         <v>12</v>
       </c>
-      <c r="S23" t="s">
+      <c r="Y23" t="s">
         <v>13</v>
       </c>
-      <c r="T23" t="s">
+      <c r="Z23" t="s">
         <v>14</v>
       </c>
-      <c r="U23" t="s">
+      <c r="AA23" t="s">
         <v>15</v>
       </c>
+      <c r="AB23" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="24" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I24">
         <v>1</v>
       </c>
@@ -3115,39 +3703,72 @@
         <v>269</v>
       </c>
       <c r="N24">
+        <v>152</v>
+      </c>
+      <c r="O24">
+        <v>146</v>
+      </c>
+      <c r="P24">
+        <v>180</v>
+      </c>
+      <c r="Q24">
         <f>LOG(J24)</f>
         <v>2.6138418218760693</v>
       </c>
-      <c r="O24">
+      <c r="R24">
         <f>LOG(K24)</f>
         <v>0.3222192947339193</v>
       </c>
-      <c r="P24">
+      <c r="S24">
         <f>LOG(L24)</f>
         <v>2.0969100130080562</v>
       </c>
-      <c r="Q24">
+      <c r="T24">
         <f>LOG(M24)</f>
         <v>2.4297522800024081</v>
       </c>
-      <c r="R24" s="1">
+      <c r="U24">
+        <f>LOG(N24)</f>
+        <v>2.1818435879447726</v>
+      </c>
+      <c r="V24">
+        <f t="shared" ref="V24:W29" si="0">LOG(O24)</f>
+        <v>2.1643528557844371</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="0"/>
+        <v>2.255272505103306</v>
+      </c>
+      <c r="X24" s="1">
         <f>J24/$I24</f>
         <v>411</v>
       </c>
-      <c r="S24" s="1">
-        <f t="shared" ref="S24:U24" si="0">K24/$I24</f>
+      <c r="Y24" s="1">
+        <f>K24/$I24</f>
         <v>2.1</v>
       </c>
-      <c r="T24" s="1">
-        <f t="shared" si="0"/>
+      <c r="Z24" s="1">
+        <f>L24/$I24</f>
         <v>125</v>
       </c>
-      <c r="U24" s="1">
-        <f t="shared" si="0"/>
+      <c r="AA24" s="1">
+        <f>M24/$I24</f>
         <v>269</v>
       </c>
+      <c r="AB24" s="1">
+        <f>N24/$I24</f>
+        <v>152</v>
+      </c>
+      <c r="AC24" s="1">
+        <f t="shared" ref="AC24:AD29" si="1">O24/$I24</f>
+        <v>146</v>
+      </c>
+      <c r="AD24" s="1">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
     </row>
-    <row r="25" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I25">
         <v>10</v>
       </c>
@@ -3164,39 +3785,72 @@
         <v>27</v>
       </c>
       <c r="N25">
+        <v>14</v>
+      </c>
+      <c r="O25">
+        <v>13</v>
+      </c>
+      <c r="P25">
+        <v>21</v>
+      </c>
+      <c r="Q25">
         <f>LOG(J25)</f>
         <v>2.3710678622717363</v>
       </c>
-      <c r="O25">
-        <f t="shared" ref="O25:Q29" si="1">LOG(K25)</f>
+      <c r="R25">
+        <f>LOG(K25)</f>
         <v>1.3222192947339193</v>
       </c>
-      <c r="P25">
+      <c r="S25">
+        <f>LOG(L25)</f>
+        <v>2.271841606536499</v>
+      </c>
+      <c r="T25">
+        <f t="shared" ref="T25:T29" si="2">LOG(M25)</f>
+        <v>1.4313637641589874</v>
+      </c>
+      <c r="U25">
+        <f t="shared" ref="U25:U29" si="3">LOG(N25)</f>
+        <v>1.146128035678238</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="0"/>
+        <v>1.1139433523068367</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="0"/>
+        <v>1.3222192947339193</v>
+      </c>
+      <c r="X25" s="1">
+        <f>J25/I25</f>
+        <v>23.5</v>
+      </c>
+      <c r="Y25" s="1">
+        <f>K25/$I25</f>
+        <v>2.1</v>
+      </c>
+      <c r="Z25" s="1">
+        <f>L25/$I25</f>
+        <v>18.7</v>
+      </c>
+      <c r="AA25" s="1">
+        <f t="shared" ref="AA25:AA29" si="4">M25/$I25</f>
+        <v>2.7</v>
+      </c>
+      <c r="AB25" s="1">
+        <f>N25/$I25</f>
+        <v>1.4</v>
+      </c>
+      <c r="AC25" s="1">
         <f t="shared" si="1"/>
-        <v>2.271841606536499</v>
-      </c>
-      <c r="Q25">
+        <v>1.3</v>
+      </c>
+      <c r="AD25" s="1">
         <f t="shared" si="1"/>
-        <v>1.4313637641589874</v>
-      </c>
-      <c r="R25" s="1">
-        <f t="shared" ref="R25:R29" si="2">J25/I25</f>
-        <v>23.5</v>
-      </c>
-      <c r="S25" s="1">
-        <f t="shared" ref="S25:S29" si="3">K25/$I25</f>
         <v>2.1</v>
       </c>
-      <c r="T25" s="1">
-        <f t="shared" ref="T25:T29" si="4">L25/$I25</f>
-        <v>18.7</v>
-      </c>
-      <c r="U25" s="1">
-        <f t="shared" ref="U25:U29" si="5">M25/$I25</f>
-        <v>2.7</v>
-      </c>
     </row>
-    <row r="26" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I26">
         <v>100</v>
       </c>
@@ -3214,39 +3868,72 @@
         <v>17</v>
       </c>
       <c r="N26">
+        <v>169</v>
+      </c>
+      <c r="O26">
+        <v>173</v>
+      </c>
+      <c r="P26">
+        <v>118</v>
+      </c>
+      <c r="Q26">
         <f>LOG(J26)</f>
         <v>3.1989318699322089</v>
       </c>
-      <c r="O26">
+      <c r="R26">
+        <f>LOG(K26)</f>
+        <v>3.3710678622717363</v>
+      </c>
+      <c r="S26">
+        <f>LOG(L26)</f>
+        <v>3.1983821300082944</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="2"/>
+        <v>1.2304489213782739</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="3"/>
+        <v>2.2278867046136734</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="0"/>
+        <v>2.2380461031287955</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="0"/>
+        <v>2.0718820073061255</v>
+      </c>
+      <c r="X26" s="1">
+        <f>J26/I26</f>
+        <v>15.81</v>
+      </c>
+      <c r="Y26" s="1">
+        <f>K26/$I26</f>
+        <v>23.5</v>
+      </c>
+      <c r="Z26" s="1">
+        <f>L26/$I26</f>
+        <v>15.79</v>
+      </c>
+      <c r="AA26" s="1">
+        <f t="shared" si="4"/>
+        <v>0.17</v>
+      </c>
+      <c r="AB26" s="1">
+        <f>N26/$I26</f>
+        <v>1.69</v>
+      </c>
+      <c r="AC26" s="1">
         <f t="shared" si="1"/>
-        <v>3.3710678622717363</v>
-      </c>
-      <c r="P26">
+        <v>1.73</v>
+      </c>
+      <c r="AD26" s="1">
         <f t="shared" si="1"/>
-        <v>3.1983821300082944</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="1"/>
-        <v>1.2304489213782739</v>
-      </c>
-      <c r="R26" s="1">
-        <f t="shared" si="2"/>
-        <v>15.81</v>
-      </c>
-      <c r="S26" s="1">
-        <f t="shared" si="3"/>
-        <v>23.5</v>
-      </c>
-      <c r="T26" s="1">
-        <f t="shared" si="4"/>
-        <v>15.79</v>
-      </c>
-      <c r="U26" s="1">
-        <f t="shared" si="5"/>
-        <v>0.17</v>
+        <v>1.18</v>
       </c>
     </row>
-    <row r="27" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I27">
         <v>1000</v>
       </c>
@@ -3264,39 +3951,72 @@
         <v>61</v>
       </c>
       <c r="N27">
+        <v>1949</v>
+      </c>
+      <c r="O27">
+        <v>1312</v>
+      </c>
+      <c r="P27">
+        <v>1323</v>
+      </c>
+      <c r="Q27">
         <f>LOG(J27)</f>
         <v>4.295083059251656</v>
       </c>
-      <c r="O27">
+      <c r="R27">
+        <f>LOG(K27)</f>
+        <v>4.3710678622717358</v>
+      </c>
+      <c r="S27">
+        <f>LOG(L27)</f>
+        <v>4.224895470849483</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="2"/>
+        <v>1.7853298350107671</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="3"/>
+        <v>3.2898118391176214</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="0"/>
+        <v>3.1179338350396413</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="0"/>
+        <v>3.1215598441875008</v>
+      </c>
+      <c r="X27" s="1">
+        <f>J27/I27</f>
+        <v>19.728000000000002</v>
+      </c>
+      <c r="Y27" s="1">
+        <f>K27/$I27</f>
+        <v>23.5</v>
+      </c>
+      <c r="Z27" s="1">
+        <f>L27/$I27</f>
+        <v>16.783999999999999</v>
+      </c>
+      <c r="AA27" s="1">
+        <f t="shared" si="4"/>
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="AB27" s="1">
+        <f>N27/$I27</f>
+        <v>1.9490000000000001</v>
+      </c>
+      <c r="AC27" s="1">
         <f t="shared" si="1"/>
-        <v>4.3710678622717358</v>
-      </c>
-      <c r="P27">
+        <v>1.3120000000000001</v>
+      </c>
+      <c r="AD27" s="1">
         <f t="shared" si="1"/>
-        <v>4.224895470849483</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="1"/>
-        <v>1.7853298350107671</v>
-      </c>
-      <c r="R27" s="1">
-        <f t="shared" si="2"/>
-        <v>19.728000000000002</v>
-      </c>
-      <c r="S27" s="1">
-        <f t="shared" si="3"/>
-        <v>23.5</v>
-      </c>
-      <c r="T27" s="1">
-        <f t="shared" si="4"/>
-        <v>16.783999999999999</v>
-      </c>
-      <c r="U27" s="1">
-        <f t="shared" si="5"/>
-        <v>6.0999999999999999E-2</v>
+        <v>1.323</v>
       </c>
     </row>
-    <row r="28" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I28">
         <v>10000</v>
       </c>
@@ -3304,7 +4024,7 @@
         <v>172795</v>
       </c>
       <c r="K28">
-        <f t="shared" ref="K28:K29" si="6">K27*10</f>
+        <f t="shared" ref="K28:K29" si="5">K27*10</f>
         <v>235000</v>
       </c>
       <c r="L28">
@@ -3314,39 +4034,72 @@
         <v>1121</v>
       </c>
       <c r="N28">
+        <v>10667</v>
+      </c>
+      <c r="O28">
+        <v>9744</v>
+      </c>
+      <c r="P28">
+        <v>10227</v>
+      </c>
+      <c r="Q28">
         <f>LOG(J28)</f>
         <v>5.237531171569807</v>
       </c>
-      <c r="O28">
+      <c r="R28">
+        <f>LOG(K28)</f>
+        <v>5.3710678622717358</v>
+      </c>
+      <c r="S28">
+        <f>LOG(L28)</f>
+        <v>5.2331383122024064</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="2"/>
+        <v>3.0496056125949731</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="3"/>
+        <v>4.0280422950907493</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="0"/>
+        <v>3.9887372752888002</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="0"/>
+        <v>4.009748255948554</v>
+      </c>
+      <c r="X28" s="1">
+        <f>J28/I28</f>
+        <v>17.279499999999999</v>
+      </c>
+      <c r="Y28" s="1">
+        <f>K28/$I28</f>
+        <v>23.5</v>
+      </c>
+      <c r="Z28" s="1">
+        <f>L28/$I28</f>
+        <v>17.105599999999999</v>
+      </c>
+      <c r="AA28" s="1">
+        <f t="shared" si="4"/>
+        <v>0.11210000000000001</v>
+      </c>
+      <c r="AB28" s="1">
+        <f>N28/$I28</f>
+        <v>1.0667</v>
+      </c>
+      <c r="AC28" s="1">
         <f t="shared" si="1"/>
-        <v>5.3710678622717358</v>
-      </c>
-      <c r="P28">
+        <v>0.97440000000000004</v>
+      </c>
+      <c r="AD28" s="1">
         <f t="shared" si="1"/>
-        <v>5.2331383122024064</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="1"/>
-        <v>3.0496056125949731</v>
-      </c>
-      <c r="R28" s="1">
-        <f t="shared" si="2"/>
-        <v>17.279499999999999</v>
-      </c>
-      <c r="S28" s="1">
-        <f t="shared" si="3"/>
-        <v>23.5</v>
-      </c>
-      <c r="T28" s="1">
-        <f t="shared" si="4"/>
-        <v>17.105599999999999</v>
-      </c>
-      <c r="U28" s="1">
-        <f t="shared" si="5"/>
-        <v>0.11210000000000001</v>
+        <v>1.0226999999999999</v>
       </c>
     </row>
-    <row r="29" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I29">
         <v>100000</v>
       </c>
@@ -3354,7 +4107,7 @@
         <v>2091718</v>
       </c>
       <c r="K29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>2350000</v>
       </c>
       <c r="L29">
@@ -3364,64 +4117,121 @@
         <v>18221</v>
       </c>
       <c r="N29">
+        <v>141592</v>
+      </c>
+      <c r="O29">
+        <v>113418</v>
+      </c>
+      <c r="P29">
+        <v>118217</v>
+      </c>
+      <c r="Q29">
         <f>LOG(J29)</f>
         <v>6.3205031336851318</v>
       </c>
-      <c r="O29">
+      <c r="R29">
+        <f>LOG(K29)</f>
+        <v>6.3710678622717358</v>
+      </c>
+      <c r="S29">
+        <f>LOG(L29)</f>
+        <v>6.2153411481740353</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="2"/>
+        <v>4.2605722081234925</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="3"/>
+        <v>5.1510387162491984</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="0"/>
+        <v>5.0546819847184326</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="0"/>
+        <v>5.0726799340352233</v>
+      </c>
+      <c r="X29" s="1">
+        <f>J29/I29</f>
+        <v>20.917179999999998</v>
+      </c>
+      <c r="Y29" s="1">
+        <f>K29/$I29</f>
+        <v>23.5</v>
+      </c>
+      <c r="Z29" s="1">
+        <f>L29/$I29</f>
+        <v>16.418790000000001</v>
+      </c>
+      <c r="AA29" s="1">
+        <f t="shared" si="4"/>
+        <v>0.18221000000000001</v>
+      </c>
+      <c r="AB29" s="1">
+        <f>N29/$I29</f>
+        <v>1.4159200000000001</v>
+      </c>
+      <c r="AC29" s="1">
         <f t="shared" si="1"/>
-        <v>6.3710678622717358</v>
-      </c>
-      <c r="P29">
+        <v>1.13418</v>
+      </c>
+      <c r="AD29" s="1">
         <f t="shared" si="1"/>
-        <v>6.2153411481740353</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="1"/>
-        <v>4.2605722081234925</v>
-      </c>
-      <c r="R29" s="1">
-        <f t="shared" si="2"/>
-        <v>20.917179999999998</v>
-      </c>
-      <c r="S29" s="1">
-        <f t="shared" si="3"/>
+        <v>1.1821699999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="9:30" x14ac:dyDescent="0.25">
+      <c r="X30" s="1">
+        <f>MEDIAN(X24:X29)</f>
+        <v>20.322589999999998</v>
+      </c>
+      <c r="Y30" s="1">
+        <f t="shared" ref="Y30:AB30" si="6">MEDIAN(Y24:Y29)</f>
         <v>23.5</v>
       </c>
-      <c r="T29" s="1">
-        <f t="shared" si="4"/>
-        <v>16.418790000000001</v>
-      </c>
-      <c r="U29" s="1">
-        <f t="shared" si="5"/>
-        <v>0.18221000000000001</v>
+      <c r="Z30" s="1">
+        <f t="shared" si="6"/>
+        <v>16.944800000000001</v>
+      </c>
+      <c r="AA30" s="1">
+        <f t="shared" si="6"/>
+        <v>0.17610500000000001</v>
+      </c>
+      <c r="AB30" s="1">
+        <f t="shared" si="6"/>
+        <v>1.5529600000000001</v>
+      </c>
+      <c r="AC30" s="1">
+        <f t="shared" ref="AC30:AD30" si="7">MEDIAN(AC24:AC29)</f>
+        <v>1.306</v>
+      </c>
+      <c r="AD30" s="1">
+        <f t="shared" si="7"/>
+        <v>1.2525849999999998</v>
       </c>
     </row>
-    <row r="30" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="R30" s="1">
-        <f>MEDIAN(R24:R29)</f>
-        <v>20.322589999999998</v>
-      </c>
-      <c r="S30" s="1">
-        <f t="shared" ref="S30:U30" si="7">MEDIAN(S24:S29)</f>
-        <v>23.5</v>
-      </c>
-      <c r="T30" s="1">
-        <f t="shared" si="7"/>
-        <v>16.944800000000001</v>
-      </c>
-      <c r="U30" s="1">
-        <f t="shared" si="7"/>
-        <v>0.17610500000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="T31" s="1">
-        <f>$R$30/T30</f>
+    <row r="31" spans="9:30" x14ac:dyDescent="0.25">
+      <c r="Z31" s="1">
+        <f>$X$30/Z30</f>
         <v>1.1993408007176241</v>
       </c>
-      <c r="U31" s="1">
-        <f>$R$30/U30</f>
+      <c r="AA31" s="1">
+        <f>$X$30/AA30</f>
         <v>115.40041452542515</v>
+      </c>
+      <c r="AB31" s="1">
+        <f>$X$30/AB30</f>
+        <v>13.08635766536163</v>
+      </c>
+      <c r="AC31" s="1">
+        <f t="shared" ref="AC31:AD31" si="8">$X$30/AC30</f>
+        <v>15.560941807044408</v>
+      </c>
+      <c r="AD31" s="1">
+        <f t="shared" si="8"/>
+        <v>16.22451969327431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix the graph a bit
</commit_message>
<xml_diff>
--- a/PerformanceGraphs.xlsx
+++ b/PerformanceGraphs.xlsx
@@ -582,6 +582,63 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4.9125196349870226</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ReadTests!$W$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Log(SQLCE Bulk)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>ReadTests!$W$24:$W$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4313637641589874</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3010299956639812</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.568201724066995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5705429398818973</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4104397862103464</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.3522404201822305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2919,8 +2976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="I20:AD31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L5" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>